<commit_message>
object deletion handling, save to binary file, customer times and renaming
added flag instead of skipping frame when an object is to be
deleted:::writes objects to binary file (customer%d.bin):::records
times objects set to track and untracked:::some renaming
</commit_message>
<xml_diff>
--- a/polynomial equation for object sizes.xlsx
+++ b/polynomial equation for object sizes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,11 +195,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2069361016"/>
-        <c:axId val="2069364088"/>
+        <c:axId val="2111474792"/>
+        <c:axId val="2111477784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2069361016"/>
+        <c:axId val="2111474792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -209,12 +209,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069364088"/>
+        <c:crossAx val="2111477784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2069364088"/>
+        <c:axId val="2111477784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -225,7 +225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069361016"/>
+        <c:crossAx val="2111474792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -326,6 +326,11 @@
               <c:numFmt formatCode="0.00000000000000E+00" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet2!$B$6:$B$27</c:f>
@@ -483,11 +488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2069439976"/>
-        <c:axId val="2069442920"/>
+        <c:axId val="2109036584"/>
+        <c:axId val="2109033608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2069439976"/>
+        <c:axId val="2109036584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,12 +502,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069442920"/>
+        <c:crossAx val="2109033608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2069442920"/>
+        <c:axId val="2109033608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,7 +518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069439976"/>
+        <c:crossAx val="2109036584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -531,6 +536,211 @@
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="0" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="3">
+                  <c:v>311.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>299.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>304.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>322.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>368.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>379.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2111877896"/>
+        <c:axId val="2124804696"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2111877896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2124804696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2124804696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2111877896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -588,6 +798,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -979,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
@@ -1425,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1638,6 +1883,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>